<commit_message>
German version, updated categories
</commit_message>
<xml_diff>
--- a/_templates/Predictive-Maintenance-Board/Sensor_Data.xlsx
+++ b/_templates/Predictive-Maintenance-Board/Sensor_Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tobiashaas/git/peakboard-templates/_templates/Predictive-Maintainance-Board/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tobiashaas/git/peakboard-templates/_templates/Predictive-Maintenance-Board/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE877C42-E60C-5E47-AB6E-D9120126BD32}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C990CA9-BF2B-894E-BDDC-22BD350B01F3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-54300" yWindow="-4160" windowWidth="42280" windowHeight="28600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1400" yWindow="460" windowWidth="35860" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="653" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="653" uniqueCount="147">
   <si>
     <t>date</t>
   </si>
@@ -320,6 +320,150 @@
   </si>
   <si>
     <t>0.43</t>
+  </si>
+  <si>
+    <t>0.09</t>
+  </si>
+  <si>
+    <t>0.1</t>
+  </si>
+  <si>
+    <t>0.32</t>
+  </si>
+  <si>
+    <t>0.24</t>
+  </si>
+  <si>
+    <t>0.31</t>
+  </si>
+  <si>
+    <t>0.16</t>
+  </si>
+  <si>
+    <t>0.17</t>
+  </si>
+  <si>
+    <t>0.28</t>
+  </si>
+  <si>
+    <t>0.48</t>
+  </si>
+  <si>
+    <t>0.52</t>
+  </si>
+  <si>
+    <t>0.54</t>
+  </si>
+  <si>
+    <t>0.59</t>
+  </si>
+  <si>
+    <t>0.64</t>
+  </si>
+  <si>
+    <t>0.66</t>
+  </si>
+  <si>
+    <t>0.67</t>
+  </si>
+  <si>
+    <t>0.62</t>
+  </si>
+  <si>
+    <t>0.61</t>
+  </si>
+  <si>
+    <t>0.58</t>
+  </si>
+  <si>
+    <t>0.11</t>
+  </si>
+  <si>
+    <t>0.26</t>
+  </si>
+  <si>
+    <t>0.36</t>
+  </si>
+  <si>
+    <t>0.65</t>
+  </si>
+  <si>
+    <t>0.63</t>
+  </si>
+  <si>
+    <t>0.60</t>
+  </si>
+  <si>
+    <t>62.4</t>
+  </si>
+  <si>
+    <t>52.1</t>
+  </si>
+  <si>
+    <t>50.3</t>
+  </si>
+  <si>
+    <t>48.2</t>
+  </si>
+  <si>
+    <t>44.3</t>
+  </si>
+  <si>
+    <t>42.9</t>
+  </si>
+  <si>
+    <t>41.0</t>
+  </si>
+  <si>
+    <t>42.1</t>
+  </si>
+  <si>
+    <t>44.0</t>
+  </si>
+  <si>
+    <t>48.0</t>
+  </si>
+  <si>
+    <t>52.0</t>
+  </si>
+  <si>
+    <t>54.0</t>
+  </si>
+  <si>
+    <t>56.0</t>
+  </si>
+  <si>
+    <t>59.0</t>
+  </si>
+  <si>
+    <t>72.4</t>
+  </si>
+  <si>
+    <t>74.2</t>
+  </si>
+  <si>
+    <t>68.3</t>
+  </si>
+  <si>
+    <t>0.004</t>
+  </si>
+  <si>
+    <t>0.002</t>
+  </si>
+  <si>
+    <t>0.000</t>
+  </si>
+  <si>
+    <t>0.054</t>
+  </si>
+  <si>
+    <t>0.043</t>
+  </si>
+  <si>
+    <t>0.031</t>
+  </si>
+  <si>
+    <t>0.0012</t>
   </si>
 </sst>
 </file>
@@ -678,8 +822,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W171"/>
   <sheetViews>
-    <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" topLeftCell="G1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -792,7 +936,7 @@
         <v>10</v>
       </c>
       <c r="K2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="L2" t="s">
         <v>19</v>
@@ -810,7 +954,7 @@
         <v>53</v>
       </c>
       <c r="Q2" t="s">
-        <v>9</v>
+        <v>90</v>
       </c>
       <c r="R2" t="s">
         <v>81</v>
@@ -854,7 +998,7 @@
         <v>17</v>
       </c>
       <c r="H3" t="s">
-        <v>53</v>
+        <v>141</v>
       </c>
       <c r="I3" t="s">
         <v>53</v>
@@ -881,13 +1025,13 @@
         <v>53</v>
       </c>
       <c r="Q3" t="s">
-        <v>94</v>
+        <v>104</v>
       </c>
       <c r="R3" t="s">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="S3" t="s">
-        <v>15</v>
+        <v>123</v>
       </c>
       <c r="T3" t="s">
         <v>16</v>
@@ -934,7 +1078,7 @@
         <v>2</v>
       </c>
       <c r="K4" t="s">
-        <v>11</v>
+        <v>81</v>
       </c>
       <c r="L4" t="s">
         <v>18</v>
@@ -952,10 +1096,10 @@
         <v>53</v>
       </c>
       <c r="Q4" t="s">
-        <v>53</v>
+        <v>92</v>
       </c>
       <c r="R4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="S4" t="s">
         <v>18</v>
@@ -1005,7 +1149,7 @@
         <v>13</v>
       </c>
       <c r="K5" t="s">
-        <v>12</v>
+        <v>81</v>
       </c>
       <c r="L5" t="s">
         <v>19</v>
@@ -1026,10 +1170,10 @@
         <v>53</v>
       </c>
       <c r="R5" t="s">
-        <v>12</v>
+        <v>88</v>
       </c>
       <c r="S5" t="s">
-        <v>19</v>
+        <v>124</v>
       </c>
       <c r="T5" t="s">
         <v>26</v>
@@ -1067,7 +1211,7 @@
         <v>31</v>
       </c>
       <c r="H6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="I6" t="s">
         <v>53</v>
@@ -1088,19 +1232,19 @@
         <v>31</v>
       </c>
       <c r="O6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="P6" t="s">
         <v>53</v>
       </c>
       <c r="Q6" t="s">
+        <v>102</v>
+      </c>
+      <c r="R6" t="s">
         <v>2</v>
       </c>
-      <c r="R6" t="s">
-        <v>13</v>
-      </c>
       <c r="S6" t="s">
-        <v>20</v>
+        <v>125</v>
       </c>
       <c r="T6" t="s">
         <v>84</v>
@@ -1109,7 +1253,7 @@
         <v>31</v>
       </c>
       <c r="V6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="W6" t="s">
         <v>53</v>
@@ -1138,7 +1282,7 @@
         <v>32</v>
       </c>
       <c r="H7" t="s">
-        <v>7</v>
+        <v>53</v>
       </c>
       <c r="I7" t="s">
         <v>53</v>
@@ -1147,7 +1291,7 @@
         <v>2</v>
       </c>
       <c r="K7" t="s">
-        <v>14</v>
+        <v>100</v>
       </c>
       <c r="L7" t="s">
         <v>21</v>
@@ -1159,19 +1303,19 @@
         <v>32</v>
       </c>
       <c r="O7" t="s">
-        <v>7</v>
+        <v>53</v>
       </c>
       <c r="P7" t="s">
         <v>53</v>
       </c>
       <c r="Q7" t="s">
-        <v>3</v>
+        <v>117</v>
       </c>
       <c r="R7" t="s">
-        <v>14</v>
+        <v>102</v>
       </c>
       <c r="S7" t="s">
-        <v>21</v>
+        <v>126</v>
       </c>
       <c r="T7" t="s">
         <v>21</v>
@@ -1180,7 +1324,7 @@
         <v>32</v>
       </c>
       <c r="V7" t="s">
-        <v>7</v>
+        <v>53</v>
       </c>
       <c r="W7" t="s">
         <v>53</v>
@@ -1209,7 +1353,7 @@
         <v>33</v>
       </c>
       <c r="H8" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="I8" t="s">
         <v>53</v>
@@ -1230,19 +1374,19 @@
         <v>33</v>
       </c>
       <c r="O8" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="P8" t="s">
         <v>53</v>
       </c>
       <c r="Q8" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="R8" t="s">
         <v>2</v>
       </c>
       <c r="S8" t="s">
-        <v>22</v>
+        <v>127</v>
       </c>
       <c r="T8" t="s">
         <v>85</v>
@@ -1251,7 +1395,7 @@
         <v>33</v>
       </c>
       <c r="V8" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="W8" t="s">
         <v>53</v>
@@ -1283,10 +1427,10 @@
         <v>53</v>
       </c>
       <c r="I9" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="J9" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="K9" t="s">
         <v>3</v>
@@ -1307,13 +1451,13 @@
         <v>53</v>
       </c>
       <c r="Q9" t="s">
-        <v>10</v>
+        <v>118</v>
       </c>
       <c r="R9" t="s">
-        <v>3</v>
+        <v>105</v>
       </c>
       <c r="S9" t="s">
-        <v>23</v>
+        <v>128</v>
       </c>
       <c r="T9" t="s">
         <v>86</v>
@@ -1354,10 +1498,10 @@
         <v>53</v>
       </c>
       <c r="I10" t="s">
-        <v>53</v>
+        <v>141</v>
       </c>
       <c r="J10" t="s">
-        <v>88</v>
+        <v>1</v>
       </c>
       <c r="K10" t="s">
         <v>9</v>
@@ -1378,13 +1522,13 @@
         <v>53</v>
       </c>
       <c r="Q10" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="R10" t="s">
-        <v>9</v>
+        <v>102</v>
       </c>
       <c r="S10" t="s">
-        <v>24</v>
+        <v>129</v>
       </c>
       <c r="T10" t="s">
         <v>36</v>
@@ -1425,13 +1569,13 @@
         <v>53</v>
       </c>
       <c r="I11" t="s">
-        <v>54</v>
+        <v>141</v>
       </c>
       <c r="J11" t="s">
         <v>9</v>
       </c>
       <c r="K11" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="L11" t="s">
         <v>25</v>
@@ -1443,19 +1587,19 @@
         <v>36</v>
       </c>
       <c r="O11" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="P11" t="s">
-        <v>54</v>
+        <v>141</v>
       </c>
       <c r="Q11" t="s">
-        <v>2</v>
+        <v>90</v>
       </c>
       <c r="R11" t="s">
-        <v>10</v>
+        <v>106</v>
       </c>
       <c r="S11" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="T11" t="s">
         <v>37</v>
@@ -1467,7 +1611,7 @@
         <v>53</v>
       </c>
       <c r="W11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.15">
@@ -1502,7 +1646,7 @@
         <v>92</v>
       </c>
       <c r="K12" t="s">
-        <v>9</v>
+        <v>99</v>
       </c>
       <c r="L12" t="s">
         <v>26</v>
@@ -1514,19 +1658,19 @@
         <v>37</v>
       </c>
       <c r="O12" t="s">
-        <v>53</v>
+        <v>140</v>
       </c>
       <c r="P12" t="s">
         <v>7</v>
       </c>
       <c r="Q12" t="s">
-        <v>3</v>
+        <v>118</v>
       </c>
       <c r="R12" t="s">
-        <v>9</v>
+        <v>102</v>
       </c>
       <c r="S12" t="s">
-        <v>26</v>
+        <v>129</v>
       </c>
       <c r="T12" t="s">
         <v>38</v>
@@ -1538,7 +1682,7 @@
         <v>53</v>
       </c>
       <c r="W12" t="s">
-        <v>7</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.15">
@@ -1573,7 +1717,7 @@
         <v>53</v>
       </c>
       <c r="K13" t="s">
-        <v>10</v>
+        <v>87</v>
       </c>
       <c r="L13" t="s">
         <v>27</v>
@@ -1585,7 +1729,7 @@
         <v>38</v>
       </c>
       <c r="O13" t="s">
-        <v>53</v>
+        <v>146</v>
       </c>
       <c r="P13" t="s">
         <v>56</v>
@@ -1594,10 +1738,10 @@
         <v>9</v>
       </c>
       <c r="R13" t="s">
-        <v>10</v>
+        <v>91</v>
       </c>
       <c r="S13" t="s">
-        <v>27</v>
+        <v>128</v>
       </c>
       <c r="T13" t="s">
         <v>20</v>
@@ -1644,7 +1788,7 @@
         <v>53</v>
       </c>
       <c r="K14" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="L14" t="s">
         <v>28</v>
@@ -1656,19 +1800,19 @@
         <v>20</v>
       </c>
       <c r="O14" t="s">
-        <v>53</v>
+        <v>141</v>
       </c>
       <c r="P14" t="s">
         <v>53</v>
       </c>
       <c r="Q14" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="R14" t="s">
-        <v>1</v>
+        <v>81</v>
       </c>
       <c r="S14" t="s">
-        <v>28</v>
+        <v>130</v>
       </c>
       <c r="T14" t="s">
         <v>4</v>
@@ -1715,7 +1859,7 @@
         <v>93</v>
       </c>
       <c r="K15" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="L15" t="s">
         <v>29</v>
@@ -1727,19 +1871,19 @@
         <v>39</v>
       </c>
       <c r="O15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="P15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="Q15" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="R15" t="s">
-        <v>11</v>
+        <v>102</v>
       </c>
       <c r="S15" t="s">
-        <v>29</v>
+        <v>131</v>
       </c>
       <c r="T15" t="s">
         <v>15</v>
@@ -1777,7 +1921,7 @@
         <v>40</v>
       </c>
       <c r="H16" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="I16" t="s">
         <v>53</v>
@@ -1786,7 +1930,7 @@
         <v>53</v>
       </c>
       <c r="K16" t="s">
-        <v>12</v>
+        <v>101</v>
       </c>
       <c r="L16" t="s">
         <v>30</v>
@@ -1798,19 +1942,19 @@
         <v>40</v>
       </c>
       <c r="O16" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="P16" t="s">
-        <v>53</v>
+        <v>141</v>
       </c>
       <c r="Q16" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="R16" t="s">
-        <v>12</v>
+        <v>103</v>
       </c>
       <c r="S16" t="s">
-        <v>30</v>
+        <v>132</v>
       </c>
       <c r="T16" t="s">
         <v>18</v>
@@ -1848,7 +1992,7 @@
         <v>41</v>
       </c>
       <c r="H17" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="I17" t="s">
         <v>53</v>
@@ -1857,7 +2001,7 @@
         <v>92</v>
       </c>
       <c r="K17" t="s">
-        <v>13</v>
+        <v>96</v>
       </c>
       <c r="L17" t="s">
         <v>31</v>
@@ -1869,19 +2013,19 @@
         <v>41</v>
       </c>
       <c r="O17" t="s">
-        <v>53</v>
+        <v>142</v>
       </c>
       <c r="P17" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="Q17" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R17" t="s">
         <v>13</v>
       </c>
       <c r="S17" t="s">
-        <v>31</v>
+        <v>133</v>
       </c>
       <c r="T17" t="s">
         <v>19</v>
@@ -1919,7 +2063,7 @@
         <v>42</v>
       </c>
       <c r="H18" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="I18" t="s">
         <v>53</v>
@@ -1943,16 +2087,16 @@
         <v>53</v>
       </c>
       <c r="P18" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="Q18" t="s">
-        <v>14</v>
+        <v>102</v>
       </c>
       <c r="R18" t="s">
         <v>14</v>
       </c>
       <c r="S18" t="s">
-        <v>32</v>
+        <v>131</v>
       </c>
       <c r="T18" t="s">
         <v>20</v>
@@ -1990,7 +2134,7 @@
         <v>43</v>
       </c>
       <c r="H19" t="s">
-        <v>53</v>
+        <v>140</v>
       </c>
       <c r="I19" t="s">
         <v>53</v>
@@ -1999,7 +2143,7 @@
         <v>1</v>
       </c>
       <c r="K19" t="s">
-        <v>2</v>
+        <v>102</v>
       </c>
       <c r="L19" t="s">
         <v>33</v>
@@ -2011,19 +2155,19 @@
         <v>43</v>
       </c>
       <c r="O19" t="s">
-        <v>53</v>
+        <v>141</v>
       </c>
       <c r="P19" t="s">
-        <v>53</v>
+        <v>141</v>
       </c>
       <c r="Q19" t="s">
-        <v>97</v>
+        <v>106</v>
       </c>
       <c r="R19" t="s">
-        <v>2</v>
+        <v>107</v>
       </c>
       <c r="S19" t="s">
-        <v>33</v>
+        <v>134</v>
       </c>
       <c r="T19" t="s">
         <v>21</v>
@@ -2035,7 +2179,7 @@
         <v>53</v>
       </c>
       <c r="W19" t="s">
-        <v>53</v>
+        <v>141</v>
       </c>
     </row>
     <row r="20" spans="1:23" x14ac:dyDescent="0.15">
@@ -2070,7 +2214,7 @@
         <v>9</v>
       </c>
       <c r="K20" t="s">
-        <v>14</v>
+        <v>103</v>
       </c>
       <c r="L20" t="s">
         <v>34</v>
@@ -2082,19 +2226,19 @@
         <v>44</v>
       </c>
       <c r="O20" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="P20" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="Q20" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="R20" t="s">
-        <v>14</v>
+        <v>108</v>
       </c>
       <c r="S20" t="s">
-        <v>34</v>
+        <v>135</v>
       </c>
       <c r="T20" t="s">
         <v>22</v>
@@ -2106,7 +2250,7 @@
         <v>53</v>
       </c>
       <c r="W20" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
     </row>
     <row r="21" spans="1:23" x14ac:dyDescent="0.15">
@@ -2141,7 +2285,7 @@
         <v>94</v>
       </c>
       <c r="K21" t="s">
-        <v>2</v>
+        <v>102</v>
       </c>
       <c r="L21" t="s">
         <v>35</v>
@@ -2159,13 +2303,13 @@
         <v>53</v>
       </c>
       <c r="Q21" t="s">
-        <v>14</v>
+        <v>95</v>
       </c>
       <c r="R21" t="s">
-        <v>2</v>
+        <v>109</v>
       </c>
       <c r="S21" t="s">
-        <v>35</v>
+        <v>136</v>
       </c>
       <c r="T21" t="s">
         <v>23</v>
@@ -2177,7 +2321,7 @@
         <v>53</v>
       </c>
       <c r="W21" t="s">
-        <v>53</v>
+        <v>141</v>
       </c>
     </row>
     <row r="22" spans="1:23" x14ac:dyDescent="0.15">
@@ -2212,7 +2356,7 @@
         <v>53</v>
       </c>
       <c r="K22" t="s">
-        <v>3</v>
+        <v>91</v>
       </c>
       <c r="L22" t="s">
         <v>36</v>
@@ -2230,13 +2374,13 @@
         <v>53</v>
       </c>
       <c r="Q22" t="s">
-        <v>13</v>
+        <v>119</v>
       </c>
       <c r="R22" t="s">
-        <v>3</v>
+        <v>110</v>
       </c>
       <c r="S22" t="s">
-        <v>36</v>
+        <v>123</v>
       </c>
       <c r="T22" t="s">
         <v>24</v>
@@ -2304,10 +2448,10 @@
         <v>14</v>
       </c>
       <c r="R23" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="S23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="T23" t="s">
         <v>25</v>
@@ -2342,7 +2486,7 @@
         <v>26</v>
       </c>
       <c r="G24" t="s">
-        <v>48</v>
+        <v>6</v>
       </c>
       <c r="H24" t="s">
         <v>53</v>
@@ -2351,7 +2495,7 @@
         <v>53</v>
       </c>
       <c r="J24" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="K24" t="s">
         <v>10</v>
@@ -2369,16 +2513,16 @@
         <v>53</v>
       </c>
       <c r="P24" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="Q24" t="s">
-        <v>2</v>
+        <v>97</v>
       </c>
       <c r="R24" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="S24" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="T24" t="s">
         <v>26</v>
@@ -2413,7 +2557,7 @@
         <v>30</v>
       </c>
       <c r="G25" t="s">
-        <v>49</v>
+        <v>17</v>
       </c>
       <c r="H25" t="s">
         <v>53</v>
@@ -2422,10 +2566,10 @@
         <v>53</v>
       </c>
       <c r="J25" t="s">
-        <v>3</v>
+        <v>87</v>
       </c>
       <c r="K25" t="s">
-        <v>9</v>
+        <v>104</v>
       </c>
       <c r="L25" t="s">
         <v>20</v>
@@ -2440,16 +2584,16 @@
         <v>53</v>
       </c>
       <c r="P25" t="s">
-        <v>53</v>
+        <v>7</v>
       </c>
       <c r="Q25" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="R25" t="s">
-        <v>9</v>
+        <v>111</v>
       </c>
       <c r="S25" t="s">
-        <v>20</v>
+        <v>137</v>
       </c>
       <c r="T25" t="s">
         <v>30</v>
@@ -2484,7 +2628,7 @@
         <v>31</v>
       </c>
       <c r="G26" t="s">
-        <v>50</v>
+        <v>26</v>
       </c>
       <c r="H26" t="s">
         <v>53</v>
@@ -2493,7 +2637,7 @@
         <v>53</v>
       </c>
       <c r="J26" t="s">
-        <v>9</v>
+        <v>94</v>
       </c>
       <c r="K26" t="s">
         <v>10</v>
@@ -2511,16 +2655,16 @@
         <v>53</v>
       </c>
       <c r="P26" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="Q26" t="s">
-        <v>9</v>
+        <v>120</v>
       </c>
       <c r="R26" t="s">
-        <v>10</v>
+        <v>112</v>
       </c>
       <c r="S26" t="s">
-        <v>4</v>
+        <v>138</v>
       </c>
       <c r="T26" t="s">
         <v>31</v>
@@ -2555,7 +2699,7 @@
         <v>32</v>
       </c>
       <c r="G27" t="s">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="H27" t="s">
         <v>53</v>
@@ -2564,10 +2708,10 @@
         <v>53</v>
       </c>
       <c r="J27" t="s">
-        <v>10</v>
+        <v>99</v>
       </c>
       <c r="K27" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="L27" t="s">
         <v>15</v>
@@ -2585,13 +2729,13 @@
         <v>53</v>
       </c>
       <c r="Q27" t="s">
-        <v>10</v>
+        <v>111</v>
       </c>
       <c r="R27" t="s">
-        <v>1</v>
+        <v>113</v>
       </c>
       <c r="S27" t="s">
-        <v>15</v>
+        <v>137</v>
       </c>
       <c r="T27" t="s">
         <v>32</v>
@@ -2600,7 +2744,7 @@
         <v>50</v>
       </c>
       <c r="V27" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="W27" t="s">
         <v>53</v>
@@ -2626,10 +2770,10 @@
         <v>33</v>
       </c>
       <c r="G28" t="s">
-        <v>51</v>
+        <v>31</v>
       </c>
       <c r="H28" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="I28" t="s">
         <v>53</v>
@@ -2638,7 +2782,7 @@
         <v>9</v>
       </c>
       <c r="K28" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="L28" t="s">
         <v>18</v>
@@ -2656,13 +2800,13 @@
         <v>53</v>
       </c>
       <c r="Q28" t="s">
-        <v>9</v>
+        <v>121</v>
       </c>
       <c r="R28" t="s">
-        <v>11</v>
+        <v>114</v>
       </c>
       <c r="S28" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="T28" t="s">
         <v>33</v>
@@ -2671,7 +2815,7 @@
         <v>51</v>
       </c>
       <c r="V28" t="s">
-        <v>53</v>
+        <v>145</v>
       </c>
       <c r="W28" t="s">
         <v>53</v>
@@ -2697,10 +2841,10 @@
         <v>34</v>
       </c>
       <c r="G29" t="s">
-        <v>52</v>
+        <v>32</v>
       </c>
       <c r="H29" t="s">
-        <v>53</v>
+        <v>7</v>
       </c>
       <c r="I29" t="s">
         <v>53</v>
@@ -2709,7 +2853,7 @@
         <v>10</v>
       </c>
       <c r="K29" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="L29" t="s">
         <v>19</v>
@@ -2727,13 +2871,13 @@
         <v>53</v>
       </c>
       <c r="Q29" t="s">
-        <v>10</v>
+        <v>122</v>
       </c>
       <c r="R29" t="s">
-        <v>12</v>
+        <v>115</v>
       </c>
       <c r="S29" t="s">
-        <v>19</v>
+        <v>137</v>
       </c>
       <c r="T29" t="s">
         <v>34</v>
@@ -2742,7 +2886,7 @@
         <v>52</v>
       </c>
       <c r="V29" t="s">
-        <v>53</v>
+        <v>144</v>
       </c>
       <c r="W29" t="s">
         <v>53</v>
@@ -2768,10 +2912,10 @@
         <v>35</v>
       </c>
       <c r="G30" t="s">
-        <v>52</v>
+        <v>33</v>
       </c>
       <c r="H30" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="I30" t="s">
         <v>53</v>
@@ -2780,7 +2924,7 @@
         <v>1</v>
       </c>
       <c r="K30" t="s">
-        <v>13</v>
+        <v>97</v>
       </c>
       <c r="L30" t="s">
         <v>20</v>
@@ -2798,13 +2942,13 @@
         <v>53</v>
       </c>
       <c r="Q30" t="s">
-        <v>1</v>
+        <v>109</v>
       </c>
       <c r="R30" t="s">
-        <v>13</v>
+        <v>109</v>
       </c>
       <c r="S30" t="s">
-        <v>20</v>
+        <v>139</v>
       </c>
       <c r="T30" t="s">
         <v>35</v>
@@ -2813,7 +2957,7 @@
         <v>52</v>
       </c>
       <c r="V30" t="s">
-        <v>53</v>
+        <v>143</v>
       </c>
       <c r="W30" t="s">
         <v>53</v>
@@ -2839,19 +2983,19 @@
         <v>36</v>
       </c>
       <c r="G31" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="H31" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="I31" t="s">
         <v>53</v>
       </c>
       <c r="J31" t="s">
+        <v>81</v>
+      </c>
+      <c r="K31" t="s">
         <v>11</v>
-      </c>
-      <c r="K31" t="s">
-        <v>14</v>
       </c>
       <c r="L31" t="s">
         <v>21</v>
@@ -2869,13 +3013,13 @@
         <v>53</v>
       </c>
       <c r="Q31" t="s">
-        <v>11</v>
+        <v>98</v>
       </c>
       <c r="R31" t="s">
-        <v>14</v>
+        <v>116</v>
       </c>
       <c r="S31" t="s">
-        <v>21</v>
+        <v>123</v>
       </c>
       <c r="T31" t="s">
         <v>36</v>
@@ -2884,7 +3028,7 @@
         <v>51</v>
       </c>
       <c r="V31" t="s">
-        <v>53</v>
+        <v>92</v>
       </c>
       <c r="W31" t="s">
         <v>53</v>

</xml_diff>